<commit_message>
feat: add validation expression for the values
</commit_message>
<xml_diff>
--- a/data/target/catalogue.xlsx
+++ b/data/target/catalogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fkelpin/git/molgenis-js-catalogue-exporter/data/target/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404A5481-8DDA-5C49-96FE-1E96EB3276DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B397350E-6457-7F4D-856F-3F3DFAAF50A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36680" yWindow="-10660" windowWidth="21560" windowHeight="16760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="148">
   <si>
     <t>name</t>
   </si>
@@ -463,6 +463,9 @@
   </si>
   <si>
     <t>times/week</t>
+  </si>
+  <si>
+    <t>$('values').isNull().or($('values').matches(/^(-?\d+\s*=\s*[^\n=]+\n)*-?\d+\s*=\s*[^\n=]+$/)).value()</t>
   </si>
 </sst>
 </file>
@@ -816,8 +819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1016,8 +1019,8 @@
       <c r="L4" t="s">
         <v>5</v>
       </c>
-      <c r="M4" t="s">
-        <v>5</v>
+      <c r="M4" t="b">
+        <v>1</v>
       </c>
       <c r="N4" t="s">
         <v>5</v>
@@ -1063,6 +1066,9 @@
       <c r="N5" t="s">
         <v>5</v>
       </c>
+      <c r="U5" t="s">
+        <v>147</v>
+      </c>
       <c r="W5" t="s">
         <v>4</v>
       </c>
@@ -1177,8 +1183,8 @@
       <c r="L8" t="s">
         <v>5</v>
       </c>
-      <c r="M8" t="s">
-        <v>5</v>
+      <c r="M8" t="b">
+        <v>1</v>
       </c>
       <c r="N8" t="s">
         <v>5</v>

</xml_diff>